<commit_message>
Source Change In Progress
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ische\Documents\Github\SESH\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD393E07-6AE8-4EFB-990D-E6B4C267D0E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4C570D-7AE5-4A4D-BD96-8B199794F155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43A60663-816A-4C42-943C-262521E3E8B4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="194">
   <si>
     <t>Code</t>
   </si>
@@ -42,26 +42,584 @@
     <t>URL</t>
   </si>
   <si>
-    <t>ETElecGen</t>
-  </si>
-  <si>
-    <t>BEISFinalConsump</t>
-  </si>
-  <si>
     <t>ESTRenHeat</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://ischerr.shinyapps.io/Reorganised/</t>
-  </si>
-  <si>
-    <t>To be added</t>
+    <t>BEISRenElec</t>
+  </si>
+  <si>
+    <t>BEISElecGen</t>
+  </si>
+  <si>
+    <t>BEISSubNatEnergy</t>
+  </si>
+  <si>
+    <t>HMRCOils</t>
+  </si>
+  <si>
+    <t>BEISSubNatElec</t>
+  </si>
+  <si>
+    <t>BEISSubNatGas</t>
+  </si>
+  <si>
+    <t>BEISLocalRoad</t>
+  </si>
+  <si>
+    <t>Renewable electricity in Scotland, Wales, Northern Ireland and the regions of England, Energy Trends, BEIS</t>
+  </si>
+  <si>
+    <t>Electricity generation and supply figures for Scotland, Wales, Northern Ireland and England, Energy Trends, BEIS</t>
+  </si>
+  <si>
+    <t>Sub-national total final energy consumption data, BEIS</t>
+  </si>
+  <si>
+    <t>Renewable Heat in Scotland, EST</t>
+  </si>
+  <si>
+    <t>Energy Consumption in the UK: end use, BEIS</t>
+  </si>
+  <si>
+    <t>Hydrocarbon Oils Bulletin, HMRC</t>
+  </si>
+  <si>
+    <t>Sub-national electricity consumption statistics, BEIS</t>
+  </si>
+  <si>
+    <t>Sub-national gas consumption statistics, BEIS</t>
+  </si>
+  <si>
+    <t>Regional and local authority road transport consumption statistics, BEIS</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/743592/ET_6.1.xls</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/853553/Regional-generation-supply-2004-2018.xls</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/833987/Sub-national-total-final-energy-consumption-statistics_2005-2017.xlsx</t>
+  </si>
+  <si>
+    <t>https://energysavingtrust.org.uk/sites/default/files/reports/Renewable%20Heat%20in%20Scotland%2C%202018%20Report.pdf</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/826726/2019_End_use_tables_2.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.uktradeinfo.com/Statistics/Tax%20and%20Duty%20Bulletins/Oils1119.xls</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/853754/Sub-national_electricity_consumption_statistics_2005-2018.xlsx</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/853430/Sub-national_gas_consumption_statistics_2005-2018.xlsx</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/812411/Road_Transport_fuel_consumption_tables_2005-2017.xlsx</t>
+  </si>
+  <si>
+    <t>Quarterly National Accounts Scotland, SG</t>
+  </si>
+  <si>
+    <t>BHRig</t>
+  </si>
+  <si>
+    <t>CASEnSwitch</t>
+  </si>
+  <si>
+    <t>BEISAnnualElec</t>
+  </si>
+  <si>
+    <t>BEISUnitElec</t>
+  </si>
+  <si>
+    <t>BEISUnitGas</t>
+  </si>
+  <si>
+    <t>BEISCHP</t>
+  </si>
+  <si>
+    <t>BEISDUKES</t>
+  </si>
+  <si>
+    <t>BEISDUKESBalance</t>
+  </si>
+  <si>
+    <t>BEISDUKESPower</t>
+  </si>
+  <si>
+    <t>BEISDUKESCoal</t>
+  </si>
+  <si>
+    <t>BEISElecPPM</t>
+  </si>
+  <si>
+    <t>BEISElecMeter</t>
+  </si>
+  <si>
+    <t>BEISImportExport</t>
+  </si>
+  <si>
+    <t>BEISOil</t>
+  </si>
+  <si>
+    <t>BEISHHoldEE</t>
+  </si>
+  <si>
+    <t>BEISInternationalPrices</t>
+  </si>
+  <si>
+    <t>BEISQuarterlyElecCustomers</t>
+  </si>
+  <si>
+    <t>BEISQuarterlyGasCustomers</t>
+  </si>
+  <si>
+    <t>BEISRegionRenew</t>
+  </si>
+  <si>
+    <t>BEISPaymentMethodElec</t>
+  </si>
+  <si>
+    <t>BEISPaymentMethodGas</t>
+  </si>
+  <si>
+    <t>BEISREPD</t>
+  </si>
+  <si>
+    <t>BEISRHI</t>
+  </si>
+  <si>
+    <t>BEISNonGasGrid</t>
+  </si>
+  <si>
+    <t>BEISGasCustomers</t>
+  </si>
+  <si>
+    <t>BEISSubNatFuel</t>
+  </si>
+  <si>
+    <t>BEISUKConsump</t>
+  </si>
+  <si>
+    <t>BEISNEED</t>
+  </si>
+  <si>
+    <t>BEISHeatNetwork</t>
+  </si>
+  <si>
+    <t>DFTLicenced</t>
+  </si>
+  <si>
+    <t>DFTULEVs</t>
+  </si>
+  <si>
+    <t>ElectralinkMeters</t>
+  </si>
+  <si>
+    <t>ElexonScotGen</t>
+  </si>
+  <si>
+    <t>ESTComm</t>
+  </si>
+  <si>
+    <t>EURORenEn</t>
+  </si>
+  <si>
+    <t>HMRCTrade</t>
+  </si>
+  <si>
+    <t>NGData</t>
+  </si>
+  <si>
+    <t>NGCarbonAPI</t>
+  </si>
+  <si>
+    <t>NGElecDemand</t>
+  </si>
+  <si>
+    <t>NRSHouseholds</t>
+  </si>
+  <si>
+    <t>OFGEMConsumers</t>
+  </si>
+  <si>
+    <t>OGAWells</t>
+  </si>
+  <si>
+    <t>OGUKWorkforce</t>
+  </si>
+  <si>
+    <t>ONSLowCarbon</t>
+  </si>
+  <si>
+    <t>ONSPopulation</t>
+  </si>
+  <si>
+    <t>SEOilGas</t>
+  </si>
+  <si>
+    <t>SGOilGasProd</t>
+  </si>
+  <si>
+    <t>SGOilGasCommodity</t>
+  </si>
+  <si>
+    <t>SGOilGasSatellite</t>
+  </si>
+  <si>
+    <t>SGQNAS</t>
+  </si>
+  <si>
+    <t>SGQNASSector</t>
+  </si>
+  <si>
+    <t>SGNonDomEnergy</t>
+  </si>
+  <si>
+    <t>SGEmissions</t>
+  </si>
+  <si>
+    <t>SGEmissionsPublic</t>
+  </si>
+  <si>
+    <t>SGSHCS</t>
+  </si>
+  <si>
+    <t>SGSNAP</t>
+  </si>
+  <si>
+    <t>SGGrowth</t>
+  </si>
+  <si>
+    <t>Internaitonal Rig Count, Baker Hughes</t>
+  </si>
+  <si>
+    <t>Energy switching rates, CAS</t>
+  </si>
+  <si>
+    <t>Annual domestic electricity bills, BEIS</t>
+  </si>
+  <si>
+    <t>Annual domestic gas bills, BEIS</t>
+  </si>
+  <si>
+    <t>Average variable unit costs and fixed costs for electricity for UK regions, BEIS</t>
+  </si>
+  <si>
+    <t>Average variable unit costs and fixed costs for gas for UK regions, BEIS</t>
+  </si>
+  <si>
+    <t>Combined Heat and Power in Scotland, Wales, Northern Ireland and the regions of England, Energy Trends, BEIS</t>
+  </si>
+  <si>
+    <t>Digest of UK Energy Statistics (DUKES), BEIS</t>
+  </si>
+  <si>
+    <t>Digest of UK Energy Statistics (DUKES): aggregate energy balance, BEIS</t>
+  </si>
+  <si>
+    <t>Digest of UK Energy Statistics (DUKES): power stations, BEIS</t>
+  </si>
+  <si>
+    <t>Digest of UK Energy Statistics (DUKES): output and employment from UK coal mines, BEIS</t>
+  </si>
+  <si>
+    <t>Electric prepayment meter statistics, BEIS</t>
+  </si>
+  <si>
+    <t>Electricty meter point data, BEIS</t>
+  </si>
+  <si>
+    <t>Energy Trends: Imports, exports and transfers of electricity, BEIS</t>
+  </si>
+  <si>
+    <t>Energy Trends: oil and oil products, BEIS</t>
+  </si>
+  <si>
+    <t>Household Energy Efficiency Statistics, BEIS</t>
+  </si>
+  <si>
+    <t>International domestic energy prices, BEIS</t>
+  </si>
+  <si>
+    <t>Quarterly domestic electricity customer numbers, BEIS</t>
+  </si>
+  <si>
+    <t>Quarterly domestic gas customer numbers, BEIS</t>
+  </si>
+  <si>
+    <t>Regional Renewable Statistics, BEIS</t>
+  </si>
+  <si>
+    <t>Regional variation of payment method for standard electricity, BEIS</t>
+  </si>
+  <si>
+    <t>Regional variation of payment method for gas, BEIS</t>
+  </si>
+  <si>
+    <t>Renewable Energy Planning Database, BEIS</t>
+  </si>
+  <si>
+    <t>Renewable Heat Incentive statistics, BEIS</t>
+  </si>
+  <si>
+    <t>Sub-national estimates of households not connected to the gas network, BEIS</t>
+  </si>
+  <si>
+    <t>Sub-national gas sales and numbers of customers, BEIS</t>
+  </si>
+  <si>
+    <t>Sub-national residual fuel consumption data, BEIS</t>
+  </si>
+  <si>
+    <t>National Energy Efficiency Data-Framework (NEED): impact of measures, BEIS</t>
+  </si>
+  <si>
+    <t>Heat Network Data, BEIS</t>
+  </si>
+  <si>
+    <t>Licensed vehicles, Department for Transport</t>
+  </si>
+  <si>
+    <t>ULEVs licensed, Department for Transport</t>
+  </si>
+  <si>
+    <t>Monthly Smart Meter Installs, Electralink</t>
+  </si>
+  <si>
+    <t>Scottish electricity generation by BMU, Elexon</t>
+  </si>
+  <si>
+    <t>Community and locally owned renewable energy in Scotland, EST</t>
+  </si>
+  <si>
+    <t>Share of renewable energy in gross final energy consumption, Eurostat</t>
+  </si>
+  <si>
+    <t>Regional Trade Statistics, HMRC</t>
+  </si>
+  <si>
+    <t>Data Item Explorer, National Grid</t>
+  </si>
+  <si>
+    <t>Carbon Intensity API, National Grid</t>
+  </si>
+  <si>
+    <t>Electricity demand data explorer, National Grid</t>
+  </si>
+  <si>
+    <t>Estimates of Households and Dwellings in Scotland, NRS</t>
+  </si>
+  <si>
+    <t>Information for Consumers, OFGEM</t>
+  </si>
+  <si>
+    <t>Well Data, Oil &amp; Gas Authority</t>
+  </si>
+  <si>
+    <t>Workforce Report, Oil &amp; Gas UK</t>
+  </si>
+  <si>
+    <t>Low Carbon and Renewable Energy Economy, Office for National Statistics</t>
+  </si>
+  <si>
+    <t>Population Estimates for UK, England and Wales, Scotland and Northern Ireland, ONS</t>
+  </si>
+  <si>
+    <t>Survey of International Activity in the Oil &amp; Gas Sector, Scottish Enterprise</t>
+  </si>
+  <si>
+    <t>Oil &amp; Gas Production Statistics, Scottish Government</t>
+  </si>
+  <si>
+    <t>Oil &amp; Gas Commodity Balances, Scottish Government</t>
+  </si>
+  <si>
+    <t>Oil and Gas Satellite Accounts, Scottish Government</t>
+  </si>
+  <si>
+    <t>Quarterly National Accounts Scotland - sectoral breakdown, SG</t>
+  </si>
+  <si>
+    <t>Scotland's non-domestic energy efficiency baseline</t>
+  </si>
+  <si>
+    <t>Scottish Greenhouse Gas Emissions, SG</t>
+  </si>
+  <si>
+    <t>Scottish Greenhouse Gas Emissions - public electricity and heat production emissions, SG</t>
+  </si>
+  <si>
+    <t>Scottish House Condition Survey, SG</t>
+  </si>
+  <si>
+    <t>Scottish National Accounts Project (SNAP), Scottish Government</t>
+  </si>
+  <si>
+    <t>Growth Sector Statistics, Scottish Government</t>
+  </si>
+  <si>
+    <t>https://bakerhughesrigcount.gcs-web.com/static-files/1f68e35c-cbca-488d-95e5-6223c2a7c6fb</t>
+  </si>
+  <si>
+    <t>https://www.cas.org.uk/news/new-data-shows-huge-differences-across-scotland-energy-switching-rates</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/812265/table_222.xlsx</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/766825/table_232.xls</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/812267/table_224.xlsx</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/797219/table_234.xlsx</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/834160/CHP_Regional_2018.pdf</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/840015/DUKES_2019_MASTER_COPY.pdf</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/820638/DUKES_1.1-1.3.xls</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/826561/DUKES_5.11.xls</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/820629/Chapter_2.pdf</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/793447/Local-authority-prepayment-electricity-statistics-2017.xlsx</t>
+  </si>
+  <si>
+    <t>Unpublished</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/766380/ET_5.6.xls</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/861747/ET_3.13.xls</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/852806/Headline_HEE_tables_19_DEC_2019_FINAL.xlsx</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/751143/table_561.xls</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/766836/table_241.xls</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/766839/table_251.xls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/743822/Renewable_electricity_by_Local_Authority__2014-2017.xlsx </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/790142/table_242.xlsx </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/790145/table_252.xlsx </t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/860252/renewable-energy-planning-database-december-2019.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.gov.uk/government/statistics/rhi-monthly-deployment-data-december-2019-annual-edition</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/853758/sub_national_estimate_of_properties_not_connected_to_the_gas_network_2015-2018.xlsx</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/833256/Sub-national_residual_fuel_consumption_statistics_2005-2017.xlsx</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/814483/Headline_Tables_Impact_of_Measures_Scotland_.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/739952/veh0104.ods </t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/763823/veh0132.ods</t>
+  </si>
+  <si>
+    <t>https://www.electralink.co.uk/services/energy-market-insight/monthly-smart-meter-installs/</t>
+  </si>
+  <si>
+    <t>https://energysavingtrust.org.uk/sites/default/files/Community%20and%20locally%20owned%20renewable%20energy%20in%20Scotland.%202019%20Report.pdf</t>
+  </si>
+  <si>
+    <t>https://appsso.eurostat.ec.europa.eu/nui/show.do?dataset=nrg_bal_c&amp;lang=en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.uktradeinfo.com/Statistics/BuildYourOwnTables/Pages/Table.aspx </t>
+  </si>
+  <si>
+    <t>https://www.nrscotland.gov.uk/files//statistics/household-estimates/2018/house-est-18-all-tabs.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.ofgem.gov.uk/data-portal/retail-market-indicators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ogauthority.co.uk/media/5150/copy-of-drilling-activity-current-last-updated-nov-2018.xls </t>
+  </si>
+  <si>
+    <t>https://oilandgasuk.co.uk/wp-content/uploads/2019/08/Workforce-Report-2019.pdf</t>
+  </si>
+  <si>
+    <t>https://www.ons.gov.uk/file?uri=%2feconomy%2fenvironmentalaccounts%2fdatasets%2flowcarbonandrenewableenergyeconomyfirstestimatesdataset%2fcurrent/lcreedataset2018.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.ons.gov.uk/file?uri=/peoplepopulationandcommunity/populationandmigration/populationestimates/datasets/populationestimatesforukenglandandwalesscotlandandnorthernireland/mid2017/ukmidyearestimates2017finalversion.xls</t>
+  </si>
+  <si>
+    <t>https://cdn.prgloo.com/media/download/51f2713e6429499d81fe3562c4bfc12b</t>
+  </si>
+  <si>
+    <t>https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/09/oil-and-gas-production-statistics-2018/documents/oil-and-gas-production-statistics-2018-web-tables/oil-and-gas-production-statistics-2018-web-tables/govscot%3Adocument/oil-gas-production-2018-tables.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/03/physical-commodity-balances-of-oil-gas-and-petroleum-1998-2017/documents/physical-commodity-balances/physical-commodity-balances/govscot%3Adocument/00547177.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/05/scottish-national-accounts-programme-whole-of-scotland-economic-accounts-project/documents/summary-tables-1998-2017/summary-tables-1998-2017/govscot%3Adocument/wseap-summary-tables-1998-2017.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/01/gdp-quarterly-national-accounts-for-scotland-2019-q3/documents/other-quarterly-national-accounts-summary-tables/other-quarterly-national-accounts-summary-tables/govscot%3Adocument/Other%2BQuarterly%2BNational%2BAccounts%2Bsummary%2Btables.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.gov.scot/binaries/content/documents/govscot/publications/research-and-analysis/2018/12/scotlands-non-domestic-energy-efficiency-baseline/documents/tables-charts/tables-charts/govscot%3Adocument/00544111.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/06/scottish-greenhouse-gas-emissions-2017/documents/2017-tables/2017-tables/govscot%3Adocument/2017-tables.xls</t>
+  </si>
+  <si>
+    <t>https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/06/scottish-greenhouse-gas-emissions-2017/documents/scottish-ghg-dataset-2017/scottish-ghg-dataset-2017/govscot%3Adocument/scottish-ghg-dataset-2017.xls</t>
+  </si>
+  <si>
+    <t>https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/01/scottish-house-condition-survey-2018-key-findings/documents/tables-figures/tables-figures/govscot%3Adocument/tables-figures.xlsx</t>
+  </si>
+  <si>
+    <t>https://www2.gov.scot/Resource/0054/00542815.xls</t>
+  </si>
+  <si>
+    <t>https://www2.gov.scot/Resource/0054/00549147.xlsx</t>
+  </si>
+  <si>
+    <t>BEISAnnualGas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +634,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,9 +668,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -417,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC4FEE88-173D-451B-B688-E6F98C0C30ED}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,38 +1015,785 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>73</v>
+      </c>
+      <c r="B54" t="s">
+        <v>130</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" t="s">
+        <v>131</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" t="s">
+        <v>138</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" t="s">
+        <v>139</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" t="s">
+        <v>134</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63" t="s">
+        <v>135</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" t="s">
+        <v>140</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" t="s">
+        <v>141</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C67">
+    <sortCondition ref="A2:A67"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="C43" r:id="rId1" xr:uid="{554A7BB0-3E08-4123-9AF9-2ABE6F3A0F83}"/>
+    <hyperlink ref="C26" r:id="rId2" xr:uid="{856EA285-F896-48F7-8F19-4C3A1155B06F}"/>
+    <hyperlink ref="C44" r:id="rId3" xr:uid="{4C135AF0-FA28-4024-90A2-E2EE3CE2FAD7}"/>
+    <hyperlink ref="C67" r:id="rId4" xr:uid="{B890180F-B981-4A1A-97CC-3C32FDE5F37C}"/>
+    <hyperlink ref="C46" r:id="rId5" xr:uid="{63283145-3568-46EB-ABB6-9D6BF90365A3}"/>
+    <hyperlink ref="C25" r:id="rId6" xr:uid="{3302F2E7-FA29-4A5B-9C49-AB95057FB7A8}"/>
+    <hyperlink ref="C27" r:id="rId7" xr:uid="{677EAABB-7FE5-4A9F-90AD-81A656787E20}"/>
+    <hyperlink ref="C45" r:id="rId8" xr:uid="{6B01E030-3336-4B04-9E89-90916A8A2F67}"/>
+    <hyperlink ref="C38" r:id="rId9" xr:uid="{E530B3F2-505D-41E4-A7DD-33AD1E1423E8}"/>
+    <hyperlink ref="C57" r:id="rId10" xr:uid="{DB0E5061-DAFA-4D28-A451-9696513F8F7A}"/>
+    <hyperlink ref="C5" r:id="rId11" xr:uid="{B599379D-62A9-4382-809C-2373D819B7DA}"/>
+    <hyperlink ref="C54" r:id="rId12" xr:uid="{D9C283E2-F1B5-4C2C-AAB7-335CE457E440}"/>
+    <hyperlink ref="C29" r:id="rId13" xr:uid="{D8764E94-B816-440A-A17C-F9DF135396CF}"/>
+    <hyperlink ref="C12" r:id="rId14" xr:uid="{39737BE8-4AA9-4F10-A2E1-8921545A79C3}"/>
+    <hyperlink ref="C66" r:id="rId15" xr:uid="{A9EAA8CE-415F-46DD-B5FE-578065634F33}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{D87ECA99-2A17-45A2-A0B8-5ECD13C65CDB}"/>
+    <hyperlink ref="C4" r:id="rId17" xr:uid="{D3755F34-5C25-425A-B36D-8047C7C8E747}"/>
+    <hyperlink ref="C51" r:id="rId18" xr:uid="{4F677A5B-26D5-4F5B-832F-C0AED91408B3}"/>
+    <hyperlink ref="C19" r:id="rId19" xr:uid="{ACB1F8D1-29F4-4F18-ADB7-FDE409EC40E1}"/>
+    <hyperlink ref="C61" r:id="rId20" xr:uid="{A0D70610-216F-4F27-950F-144D8E37E2B5}"/>
+    <hyperlink ref="C62" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/09/oil-and-gas-production-statistics-2018/documents/oil-and-gas-production-statistics-2018-web-tables/oil-and-gas-production-statistics-2018-web-tables/govscot%3Adocument" xr:uid="{98F9BD2A-E536-4707-BCD0-D046CCAC73DD}"/>
+    <hyperlink ref="C52" r:id="rId21" xr:uid="{D573BCF0-8FF6-4EE6-BB1A-66696E3CF271}"/>
+    <hyperlink ref="C56" r:id="rId22" xr:uid="{22602E05-EFEE-461B-BDA3-4F477AF77B52}"/>
+    <hyperlink ref="C53" r:id="rId23" xr:uid="{E27D0315-6213-460F-A16E-64A88EF2F413}"/>
+    <hyperlink ref="C63" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/05/scottish-national-accounts-programme-whole-of-scotland-economic-accounts-project/documents/summary-tables-1998-2017/summary-tables-1998-2017/govscot%3Adocument/wseap-s" xr:uid="{F6836856-11B9-44FF-B52A-4BFE477E5D66}"/>
+    <hyperlink ref="C7" r:id="rId24" xr:uid="{1FAB39C9-08C2-40F8-BFF5-EA9D14272852}"/>
+    <hyperlink ref="C55" r:id="rId25" xr:uid="{9F65E14F-F95F-4D14-BF38-38D5A175E56C}"/>
+    <hyperlink ref="C39" r:id="rId26" xr:uid="{FA42AE22-54E5-49D7-A8AA-D8D80F119CB9}"/>
+    <hyperlink ref="C59" r:id="rId27" xr:uid="{A427E7B2-E2BC-4EF5-B9B1-9CB481194374}"/>
+    <hyperlink ref="C40" r:id="rId28" xr:uid="{57A3A524-BBF2-47D6-BAEF-90D2798B753D}"/>
+    <hyperlink ref="C22" r:id="rId29" xr:uid="{BF5B0143-E3FD-44BE-B276-38D8CE4F2136}"/>
+    <hyperlink ref="C21" r:id="rId30" xr:uid="{70295F80-CB36-4205-99ED-229C22825D97}"/>
+    <hyperlink ref="C37" r:id="rId31" xr:uid="{148C2518-1FBC-4B58-9891-FFA9A6A0700A}"/>
+    <hyperlink ref="C30" r:id="rId32" xr:uid="{00F673DE-34B5-4369-8801-63B5DB64A196}"/>
+    <hyperlink ref="C35" r:id="rId33" xr:uid="{85C2CB68-C735-4375-9D25-B4EB26E44DF0}"/>
+    <hyperlink ref="C11" r:id="rId34" xr:uid="{2F93C850-4CAD-4563-93F6-F321186591BD}"/>
+    <hyperlink ref="C50" r:id="rId35" xr:uid="{6E90DFF6-1687-4CF8-A96A-67D0A5977FAC}"/>
+    <hyperlink ref="C14" r:id="rId36" xr:uid="{6F92D657-5490-4B8F-A1E1-EC61F04DA13D}"/>
+    <hyperlink ref="C60" r:id="rId37" xr:uid="{7001CAC8-8FEB-41A5-BDC1-D7504973EC9A}"/>
+    <hyperlink ref="C9" r:id="rId38" xr:uid="{C3E36E5A-412F-4A53-8ABD-EFC86EEC74E4}"/>
+    <hyperlink ref="C2" r:id="rId39" xr:uid="{33C5C0A2-B7F4-4DC6-A34D-E3BD33E7FAD1}"/>
+    <hyperlink ref="C3" r:id="rId40" xr:uid="{8697F89A-4896-471A-AEB1-B216BD522C4F}"/>
+    <hyperlink ref="C34" r:id="rId41" xr:uid="{F6E268EE-286C-4AC3-BE4A-5D91A9517FA3}"/>
+    <hyperlink ref="C8" r:id="rId42" xr:uid="{CFF81088-1EDC-4A68-AA47-E2881F091675}"/>
+    <hyperlink ref="C6" r:id="rId43" xr:uid="{B76BA9B7-82A1-4A8D-A445-7D7F86D3C093}"/>
+    <hyperlink ref="C15" r:id="rId44" xr:uid="{3743DC60-593A-43F4-9A4C-BE62851B3C46}"/>
+    <hyperlink ref="C23" r:id="rId45" xr:uid="{67674276-2916-43BC-BED8-7C73B2ABF013}"/>
+    <hyperlink ref="C24" r:id="rId46" xr:uid="{E4E3CF03-750F-4AC0-93CA-EA8E698074DD}"/>
+    <hyperlink ref="C28" r:id="rId47" xr:uid="{CE024799-1121-4030-A562-F88376E38393}"/>
+    <hyperlink ref="C32" r:id="rId48" xr:uid="{0966A0AB-F9B2-4E61-9663-831C64081062}"/>
+    <hyperlink ref="C31" r:id="rId49" xr:uid="{0F7D650D-3F75-45BD-BFB0-841F3F195CD6}"/>
+    <hyperlink ref="C33" r:id="rId50" xr:uid="{1BE19B78-B19D-4BED-97BE-D9181565AF64}"/>
+    <hyperlink ref="C42" r:id="rId51" xr:uid="{238AA3D9-186C-44A9-ABA9-2463219A62E8}"/>
+    <hyperlink ref="C64" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/01/gdp-quarterly-national-accounts-for-scotland-2019-q3/documents/other-quarterly-national-accounts-summary-tables/other-quarterly-national-accounts-summary-tables/govsco" xr:uid="{807C7CE0-CE35-493D-9ED5-C8BB51538F06}"/>
+    <hyperlink ref="C58" r:id="rId52" xr:uid="{D03659B1-635B-4840-9A2A-0F745097A4E4}"/>
+    <hyperlink ref="C18" r:id="rId53" xr:uid="{F256E6CF-91E1-4BD2-9EFB-CFBDE7C48C86}"/>
+    <hyperlink ref="C20" r:id="rId54" xr:uid="{A4E0F597-97B5-4409-9FFA-D94402916AB2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Source Updates and Corrections
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ische\Documents\Github\SESH\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4C570D-7AE5-4A4D-BD96-8B199794F155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF37763-AEBB-47C8-A37F-6063CD0580A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43A60663-816A-4C42-943C-262521E3E8B4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="197">
   <si>
     <t>Code</t>
   </si>
@@ -66,33 +66,6 @@
     <t>BEISLocalRoad</t>
   </si>
   <si>
-    <t>Renewable electricity in Scotland, Wales, Northern Ireland and the regions of England, Energy Trends, BEIS</t>
-  </si>
-  <si>
-    <t>Electricity generation and supply figures for Scotland, Wales, Northern Ireland and England, Energy Trends, BEIS</t>
-  </si>
-  <si>
-    <t>Sub-national total final energy consumption data, BEIS</t>
-  </si>
-  <si>
-    <t>Renewable Heat in Scotland, EST</t>
-  </si>
-  <si>
-    <t>Energy Consumption in the UK: end use, BEIS</t>
-  </si>
-  <si>
-    <t>Hydrocarbon Oils Bulletin, HMRC</t>
-  </si>
-  <si>
-    <t>Sub-national electricity consumption statistics, BEIS</t>
-  </si>
-  <si>
-    <t>Sub-national gas consumption statistics, BEIS</t>
-  </si>
-  <si>
-    <t>Regional and local authority road transport consumption statistics, BEIS</t>
-  </si>
-  <si>
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/743592/ET_6.1.xls</t>
   </si>
   <si>
@@ -120,9 +93,6 @@
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/812411/Road_Transport_fuel_consumption_tables_2005-2017.xlsx</t>
   </si>
   <si>
-    <t>Quarterly National Accounts Scotland, SG</t>
-  </si>
-  <si>
     <t>BHRig</t>
   </si>
   <si>
@@ -294,174 +264,6 @@
     <t>SGGrowth</t>
   </si>
   <si>
-    <t>Internaitonal Rig Count, Baker Hughes</t>
-  </si>
-  <si>
-    <t>Energy switching rates, CAS</t>
-  </si>
-  <si>
-    <t>Annual domestic electricity bills, BEIS</t>
-  </si>
-  <si>
-    <t>Annual domestic gas bills, BEIS</t>
-  </si>
-  <si>
-    <t>Average variable unit costs and fixed costs for electricity for UK regions, BEIS</t>
-  </si>
-  <si>
-    <t>Average variable unit costs and fixed costs for gas for UK regions, BEIS</t>
-  </si>
-  <si>
-    <t>Combined Heat and Power in Scotland, Wales, Northern Ireland and the regions of England, Energy Trends, BEIS</t>
-  </si>
-  <si>
-    <t>Digest of UK Energy Statistics (DUKES), BEIS</t>
-  </si>
-  <si>
-    <t>Digest of UK Energy Statistics (DUKES): aggregate energy balance, BEIS</t>
-  </si>
-  <si>
-    <t>Digest of UK Energy Statistics (DUKES): power stations, BEIS</t>
-  </si>
-  <si>
-    <t>Digest of UK Energy Statistics (DUKES): output and employment from UK coal mines, BEIS</t>
-  </si>
-  <si>
-    <t>Electric prepayment meter statistics, BEIS</t>
-  </si>
-  <si>
-    <t>Electricty meter point data, BEIS</t>
-  </si>
-  <si>
-    <t>Energy Trends: Imports, exports and transfers of electricity, BEIS</t>
-  </si>
-  <si>
-    <t>Energy Trends: oil and oil products, BEIS</t>
-  </si>
-  <si>
-    <t>Household Energy Efficiency Statistics, BEIS</t>
-  </si>
-  <si>
-    <t>International domestic energy prices, BEIS</t>
-  </si>
-  <si>
-    <t>Quarterly domestic electricity customer numbers, BEIS</t>
-  </si>
-  <si>
-    <t>Quarterly domestic gas customer numbers, BEIS</t>
-  </si>
-  <si>
-    <t>Regional Renewable Statistics, BEIS</t>
-  </si>
-  <si>
-    <t>Regional variation of payment method for standard electricity, BEIS</t>
-  </si>
-  <si>
-    <t>Regional variation of payment method for gas, BEIS</t>
-  </si>
-  <si>
-    <t>Renewable Energy Planning Database, BEIS</t>
-  </si>
-  <si>
-    <t>Renewable Heat Incentive statistics, BEIS</t>
-  </si>
-  <si>
-    <t>Sub-national estimates of households not connected to the gas network, BEIS</t>
-  </si>
-  <si>
-    <t>Sub-national gas sales and numbers of customers, BEIS</t>
-  </si>
-  <si>
-    <t>Sub-national residual fuel consumption data, BEIS</t>
-  </si>
-  <si>
-    <t>National Energy Efficiency Data-Framework (NEED): impact of measures, BEIS</t>
-  </si>
-  <si>
-    <t>Heat Network Data, BEIS</t>
-  </si>
-  <si>
-    <t>Licensed vehicles, Department for Transport</t>
-  </si>
-  <si>
-    <t>ULEVs licensed, Department for Transport</t>
-  </si>
-  <si>
-    <t>Monthly Smart Meter Installs, Electralink</t>
-  </si>
-  <si>
-    <t>Scottish electricity generation by BMU, Elexon</t>
-  </si>
-  <si>
-    <t>Community and locally owned renewable energy in Scotland, EST</t>
-  </si>
-  <si>
-    <t>Share of renewable energy in gross final energy consumption, Eurostat</t>
-  </si>
-  <si>
-    <t>Regional Trade Statistics, HMRC</t>
-  </si>
-  <si>
-    <t>Data Item Explorer, National Grid</t>
-  </si>
-  <si>
-    <t>Carbon Intensity API, National Grid</t>
-  </si>
-  <si>
-    <t>Electricity demand data explorer, National Grid</t>
-  </si>
-  <si>
-    <t>Estimates of Households and Dwellings in Scotland, NRS</t>
-  </si>
-  <si>
-    <t>Information for Consumers, OFGEM</t>
-  </si>
-  <si>
-    <t>Well Data, Oil &amp; Gas Authority</t>
-  </si>
-  <si>
-    <t>Workforce Report, Oil &amp; Gas UK</t>
-  </si>
-  <si>
-    <t>Low Carbon and Renewable Energy Economy, Office for National Statistics</t>
-  </si>
-  <si>
-    <t>Population Estimates for UK, England and Wales, Scotland and Northern Ireland, ONS</t>
-  </si>
-  <si>
-    <t>Survey of International Activity in the Oil &amp; Gas Sector, Scottish Enterprise</t>
-  </si>
-  <si>
-    <t>Oil &amp; Gas Production Statistics, Scottish Government</t>
-  </si>
-  <si>
-    <t>Oil &amp; Gas Commodity Balances, Scottish Government</t>
-  </si>
-  <si>
-    <t>Oil and Gas Satellite Accounts, Scottish Government</t>
-  </si>
-  <si>
-    <t>Quarterly National Accounts Scotland - sectoral breakdown, SG</t>
-  </si>
-  <si>
-    <t>Scotland's non-domestic energy efficiency baseline</t>
-  </si>
-  <si>
-    <t>Scottish Greenhouse Gas Emissions, SG</t>
-  </si>
-  <si>
-    <t>Scottish Greenhouse Gas Emissions - public electricity and heat production emissions, SG</t>
-  </si>
-  <si>
-    <t>Scottish House Condition Survey, SG</t>
-  </si>
-  <si>
-    <t>Scottish National Accounts Project (SNAP), Scottish Government</t>
-  </si>
-  <si>
-    <t>Growth Sector Statistics, Scottish Government</t>
-  </si>
-  <si>
     <t>https://bakerhughesrigcount.gcs-web.com/static-files/1f68e35c-cbca-488d-95e5-6223c2a7c6fb</t>
   </si>
   <si>
@@ -613,6 +415,213 @@
   </si>
   <si>
     <t>BEISAnnualGas</t>
+  </si>
+  <si>
+    <t>BEIS: Annual domestic gas bills</t>
+  </si>
+  <si>
+    <t>BEIS: Annual domestic electricity bills</t>
+  </si>
+  <si>
+    <t>BEIS: Combined Heat and Power in Scotland, Wales, Northern Ireland and the regions of England, Energy Trends</t>
+  </si>
+  <si>
+    <t>BEIS: Digest of UK Energy Statistics (DUKES)</t>
+  </si>
+  <si>
+    <t>BEIS: Digest of UK Energy Statistics (DUKES): aggregate energy balance</t>
+  </si>
+  <si>
+    <t>BEIS: Digest of UK Energy Statistics (DUKES): output and employment from UK coal mines</t>
+  </si>
+  <si>
+    <t>BEIS: Digest of UK Energy Statistics (DUKES): power stations</t>
+  </si>
+  <si>
+    <t>BEIS: Electricity generation and supply figures for Scotland, Wales, Northern Ireland and England, Energy Trends</t>
+  </si>
+  <si>
+    <t>BEIS: Electricty meter point data</t>
+  </si>
+  <si>
+    <t>BEIS: Electric prepayment meter statistics</t>
+  </si>
+  <si>
+    <t>BEIS: Sub-national gas sales and numbers of customers</t>
+  </si>
+  <si>
+    <t>BEIS: Heat Network Data</t>
+  </si>
+  <si>
+    <t>BEIS: Household Energy Efficiency Statistics</t>
+  </si>
+  <si>
+    <t>BEIS: Energy Trends: Imports, exports and transfers of electricity</t>
+  </si>
+  <si>
+    <t>BEIS: International domestic energy prices</t>
+  </si>
+  <si>
+    <t>BEIS: Regional and local authority road transport consumption statistics</t>
+  </si>
+  <si>
+    <t>BEIS: National Energy Efficiency Data-Framework (NEED): impact of measures</t>
+  </si>
+  <si>
+    <t>BEIS: Sub-national estimates of households not connected to the gas network</t>
+  </si>
+  <si>
+    <t>BEIS: Energy Trends: oil and oil products</t>
+  </si>
+  <si>
+    <t>BEIS: Regional variation of payment method for standard electricity</t>
+  </si>
+  <si>
+    <t>BEIS: Regional variation of payment method for gas</t>
+  </si>
+  <si>
+    <t>BEIS: Quarterly domestic electricity customer numbers</t>
+  </si>
+  <si>
+    <t>BEIS: Quarterly domestic gas customer numbers</t>
+  </si>
+  <si>
+    <t>BEIS: Regional Renewable Statistics</t>
+  </si>
+  <si>
+    <t>BEIS: Renewable electricity in Scotland, Wales, Northern Ireland and the regions of England, Energy Trends</t>
+  </si>
+  <si>
+    <t>BEIS: Renewable Energy Planning Database</t>
+  </si>
+  <si>
+    <t>BEIS: Renewable Heat Incentive statistics</t>
+  </si>
+  <si>
+    <t>BEIS: Sub-national electricity consumption statistics</t>
+  </si>
+  <si>
+    <t>BEIS: Sub-national total final energy consumption data</t>
+  </si>
+  <si>
+    <t>BEIS: Sub-national residual fuel consumption data</t>
+  </si>
+  <si>
+    <t>BEIS: Sub-national gas consumption statistics</t>
+  </si>
+  <si>
+    <t>BEIS: Energy Consumption in the UK: end use</t>
+  </si>
+  <si>
+    <t>BEIS: Average variable unit costs and fixed costs for electricity for UK regions</t>
+  </si>
+  <si>
+    <t>BEIS: Average variable unit costs and fixed costs for gas for UK regions</t>
+  </si>
+  <si>
+    <t>Baker Hughes: Internaitonal Rig Count</t>
+  </si>
+  <si>
+    <t>CAS: Energy switching rates</t>
+  </si>
+  <si>
+    <t>Department for Transport: Licensed vehicles</t>
+  </si>
+  <si>
+    <t>Department for Transport: ULEVs licensed</t>
+  </si>
+  <si>
+    <t>Electralink: Monthly Smart Meter Installs</t>
+  </si>
+  <si>
+    <t>Elexon: Scottish electricity generation by BMU</t>
+  </si>
+  <si>
+    <t>Energy Savings Trust: Community and locally owned renewable energy in Scotland</t>
+  </si>
+  <si>
+    <t>Energy Savings Trust: Renewable Heat in Scotland</t>
+  </si>
+  <si>
+    <t>Eurostat: Share of renewable energy in gross final energy consumption</t>
+  </si>
+  <si>
+    <t>HMRC: Hydrocarbon Oils Bulletin</t>
+  </si>
+  <si>
+    <t>HMRC: Regional Trade Statistics</t>
+  </si>
+  <si>
+    <t>National Grid: Carbon Intensity API</t>
+  </si>
+  <si>
+    <t>National Grid: Data Item Explorer</t>
+  </si>
+  <si>
+    <t>National Grid: Electricity demand data explorer</t>
+  </si>
+  <si>
+    <t>NRS: Estimates of Households and Dwellings in Scotland</t>
+  </si>
+  <si>
+    <t>OFGEM: Information for Consumers</t>
+  </si>
+  <si>
+    <t>Oil &amp; Gas Authority: Well Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oil &amp; Gas UK: Workforce Report </t>
+  </si>
+  <si>
+    <t>Office for National Statistics: Low Carbon and Renewable Energy Economy</t>
+  </si>
+  <si>
+    <t>Scottish Enterprise: Survey of International Activity in the Oil &amp; Gas Sector</t>
+  </si>
+  <si>
+    <t>Scottish Government: Scottish Greenhouse Gas Emissions</t>
+  </si>
+  <si>
+    <t>Scottish Government: Scottish Greenhouse Gas Emissions - public electricity and heat production emissions</t>
+  </si>
+  <si>
+    <t>Scottish Government: Growth Sector Statistics</t>
+  </si>
+  <si>
+    <t>Scottish Government: Scotland's non-domestic energy efficiency baseline</t>
+  </si>
+  <si>
+    <t>Scottish Government: Oil &amp; Gas Commodity Balances</t>
+  </si>
+  <si>
+    <t>Office for National Statistics: Population Estimates for UK, England and Wales, Scotland and Northern Ireland</t>
+  </si>
+  <si>
+    <t>Scottish Government: Oil &amp; Gas Production Statistics</t>
+  </si>
+  <si>
+    <t>Scottish Government: Oil and Gas Satellite Accounts</t>
+  </si>
+  <si>
+    <t>Scottish Government: Quarterly National Accounts Scotland</t>
+  </si>
+  <si>
+    <t>Scottish Government: Quarterly National Accounts Scotland - sectoral breakdown</t>
+  </si>
+  <si>
+    <t>Scottish Government: Scottish House Condition Survey</t>
+  </si>
+  <si>
+    <t>Scottish Government: Scottish National Accounts Project (SNAP)</t>
+  </si>
+  <si>
+    <t>https://www.elexon.co.uk/</t>
+  </si>
+  <si>
+    <t>https://carbonintensity.org.uk/</t>
+  </si>
+  <si>
+    <t>https://www.nationalgrideso.com/balancing-data/data-finder-and-explorer</t>
   </si>
 </sst>
 </file>
@@ -993,7 +1002,7 @@
   <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,79 +1024,79 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>146</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>149</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>150</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>151</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1095,87 +1104,87 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>154</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>158</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>156</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>159</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1183,98 +1192,98 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>167</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>157</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>163</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>160</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1282,32 +1291,32 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>153</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1315,10 +1324,10 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1326,21 +1335,21 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1348,118 +1357,120 @@
         <v>9</v>
       </c>
       <c r="B32" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>160</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>147</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>161</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>148</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>143</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>163</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>144</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>164</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>171</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>172</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" s="3"/>
+        <v>167</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>173</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1467,21 +1478,21 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
+        <v>169</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>174</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1489,246 +1500,252 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>122</v>
+        <v>172</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>175</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
-      </c>
-      <c r="C47" s="3"/>
+        <v>173</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>123</v>
-      </c>
-      <c r="C48" s="3"/>
+        <v>174</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>125</v>
-      </c>
-      <c r="C49" s="3"/>
+        <v>175</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>176</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>176</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
-        <v>127</v>
+        <v>177</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>177</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>178</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>178</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>129</v>
+        <v>179</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>179</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>180</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>187</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>181</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B56" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>182</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>188</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>189</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B59" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>192</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>187</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>134</v>
+        <v>186</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>184</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>188</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>189</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>185</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>29</v>
+        <v>190</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>186</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>136</v>
+        <v>191</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B66" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>190</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B67" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>191</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1793,6 +1810,10 @@
     <hyperlink ref="C58" r:id="rId52" xr:uid="{D03659B1-635B-4840-9A2A-0F745097A4E4}"/>
     <hyperlink ref="C18" r:id="rId53" xr:uid="{F256E6CF-91E1-4BD2-9EFB-CFBDE7C48C86}"/>
     <hyperlink ref="C20" r:id="rId54" xr:uid="{A4E0F597-97B5-4409-9FFA-D94402916AB2}"/>
+    <hyperlink ref="C41" r:id="rId55" xr:uid="{3B2AAC33-EE2F-4F55-AB02-34CF0A1C590B}"/>
+    <hyperlink ref="C47" r:id="rId56" xr:uid="{6BB47E63-04A9-40F2-885E-B78C05619C21}"/>
+    <hyperlink ref="C48" r:id="rId57" xr:uid="{F2173860-7DF3-44C6-927A-0F6ACDBFF5F5}"/>
+    <hyperlink ref="C49" r:id="rId58" xr:uid="{857A1663-EE3A-4A80-93DD-3ED05824AE86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Revert "Update Sources.xlsx""
This reverts commit 7df6da3aa66808bc63b28b064c9253d550e4154d.
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48530ed5e3c44a15/Documents/GitHub/Scottish-Energy-Statistics-Hub/Structure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{6A55E799-6761-4A8D-9CC6-7690E84C63E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E30A4F69-E66D-4618-96DE-50BC821DB006}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{6A55E799-6761-4A8D-9CC6-7690E84C63E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A126281C-F080-4A1D-BF27-678F6574F993}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -633,9 +633,6 @@
     <t xml:space="preserve">https://www.gov.uk/government/statistical-data-sets/quarterly-domestic-energy-price-stastics </t>
   </si>
   <si>
-    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/875736/table_221.xlsx</t>
-  </si>
-  <si>
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/875743/table_232.xlsx</t>
   </si>
   <si>
@@ -745,6 +742,9 @@
   </si>
   <si>
     <t>BEISElecConsump</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/875737/table_222.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1239,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1274,7 +1274,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -1288,7 +1288,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>200</v>
+        <v>237</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>169</v>
@@ -1297,7 +1297,7 @@
         <v>43916</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G2" s="1">
         <f>DATE(YEAR(E2),MONTH(E2)+3,DAY(E2))</f>
@@ -1315,7 +1315,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>169</v>
@@ -1324,7 +1324,7 @@
         <v>43916</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G3" s="1">
         <f>DATE(YEAR(E3),MONTH(E3)+3,DAY(E3))</f>
@@ -1345,13 +1345,13 @@
         <v>11</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E4" s="1">
         <v>43734</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ref="G4:G10" si="0">DATE(YEAR(E4)+1,MONTH(E4),DAY(E4))</f>
@@ -1378,7 +1378,7 @@
         <v>43647</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
@@ -1405,7 +1405,7 @@
         <v>43647</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
@@ -1432,7 +1432,7 @@
         <v>43647</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
@@ -1459,7 +1459,7 @@
         <v>43647</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
@@ -1471,22 +1471,22 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>225</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>226</v>
       </c>
       <c r="E9" s="11">
         <v>43862</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G9" s="11">
         <f t="shared" si="0"/>
@@ -1513,7 +1513,7 @@
         <v>43800</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
@@ -1537,7 +1537,7 @@
         <v>43916</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H11">
         <v>2018</v>
@@ -1560,7 +1560,7 @@
         <v>43818</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G12" s="1">
         <f>DATE(YEAR(E12)+1,MONTH(E12),DAY(E12))</f>
@@ -1585,7 +1585,7 @@
         <v>43466</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13">
@@ -1600,7 +1600,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>172</v>
@@ -1609,7 +1609,7 @@
         <v>43862</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G14" s="1">
         <f>DATE(YEAR(E14),MONTH(E14)+3,DAY(E14))</f>
@@ -1627,7 +1627,7 @@
         <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>173</v>
@@ -1636,7 +1636,7 @@
         <v>43916</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G15" s="1">
         <f>DATE(YEAR(E15),MONTH(E15)+3,DAY(E15))</f>
@@ -1663,7 +1663,7 @@
         <v>43622</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G16" s="1">
         <f>DATE(YEAR(E16)+1,MONTH(E16),DAY(E16))</f>
@@ -1690,7 +1690,7 @@
         <v>43643</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G17" s="1">
         <f>DATE(YEAR(E17)+1,MONTH(E17),DAY(E17))</f>
@@ -1717,7 +1717,7 @@
         <v>43800</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G18" s="1">
         <f>DATE(YEAR(E18)+1,MONTH(E18),DAY(E18))</f>
@@ -1744,7 +1744,7 @@
         <v>43888</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" ref="G19:G25" si="1">DATE(YEAR(E19),MONTH(E19)+3,DAY(E19))</f>
@@ -1762,7 +1762,7 @@
         <v>52</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>178</v>
@@ -1771,7 +1771,7 @@
         <v>43916</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="1"/>
@@ -1789,7 +1789,7 @@
         <v>54</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>178</v>
@@ -1798,7 +1798,7 @@
         <v>43916</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="1"/>
@@ -1816,7 +1816,7 @@
         <v>56</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>199</v>
@@ -1825,7 +1825,7 @@
         <v>43916</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="1"/>
@@ -1843,7 +1843,7 @@
         <v>58</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>178</v>
@@ -1852,7 +1852,7 @@
         <v>43916</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="1"/>
@@ -1870,7 +1870,7 @@
         <v>60</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>179</v>
@@ -1879,7 +1879,7 @@
         <v>43916</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="1"/>
@@ -1897,7 +1897,7 @@
         <v>62</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>180</v>
@@ -1906,7 +1906,7 @@
         <v>43922</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="1"/>
@@ -1924,7 +1924,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>181</v>
@@ -1933,7 +1933,7 @@
         <v>43922</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G26" s="1">
         <f>DATE(YEAR(E26),MONTH(E26)+1,DAY(E26))</f>
@@ -1960,7 +1960,7 @@
         <v>43800</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G27" s="1">
         <f>DATE(YEAR(E27)+1,MONTH(E27),DAY(E27))</f>
@@ -1987,7 +1987,7 @@
         <v>43709</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G28" s="1">
         <f>DATE(YEAR(E28)+1,MONTH(E28),DAY(E28))</f>
@@ -2014,7 +2014,7 @@
         <v>43734</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G29" s="1">
         <f>DATE(YEAR(E29)+1,MONTH(E29),DAY(E29))</f>
@@ -2041,7 +2041,7 @@
         <v>43800</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G30" s="1">
         <f>DATE(YEAR(E30)+1,MONTH(E30),DAY(E30))</f>
@@ -2068,7 +2068,7 @@
         <v>43647</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G31" s="1">
         <f>DATE(YEAR(E31)+1,MONTH(E31),DAY(E31))</f>
@@ -2095,7 +2095,7 @@
         <v>43891</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G32" s="1">
         <f>DATE(YEAR(E32),MONTH(E32)+3,DAY(E32))</f>
@@ -2122,7 +2122,7 @@
         <v>43892</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G33" s="1">
         <f>DATE(YEAR(E33),MONTH(E33)+3,DAY(E33))</f>
@@ -2149,7 +2149,7 @@
         <v>43800</v>
       </c>
       <c r="F34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G34" s="1">
         <v>43922</v>
@@ -2169,13 +2169,13 @@
         <v>162</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E35" s="1">
         <v>43862</v>
       </c>
       <c r="F35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G35" s="1">
         <f>DATE(YEAR(E35),MONTH(E35)+3,DAY(E35))</f>
@@ -2202,7 +2202,7 @@
         <v>43800</v>
       </c>
       <c r="F36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G36" s="1">
         <v>43922</v>
@@ -2222,13 +2222,13 @@
         <v>93</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E37" s="1">
         <v>43916</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G37" s="1">
         <f>DATE(YEAR(E37),MONTH(E37)+1,DAY(E37))</f>
@@ -2246,7 +2246,7 @@
         <v>95</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>96</v>
@@ -2255,7 +2255,7 @@
         <v>43831</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G38" s="1">
         <f>DATE(YEAR(E38)+1,MONTH(E38),DAY(E38))</f>
@@ -2276,13 +2276,13 @@
         <v>99</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E39" s="1">
         <v>43831</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G39" s="1">
         <f>DATE(YEAR(E39)+1,MONTH(E39),DAY(E39))</f>
@@ -2309,7 +2309,7 @@
         <v>43739</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G40" s="1">
         <f>DATE(YEAR(E40)+1,MONTH(E40),DAY(E40))</f>
@@ -2330,13 +2330,13 @@
         <v>105</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E41" s="1">
         <v>43831</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G41" s="1">
         <f>DATE(YEAR(E41),MONTH(E41)+3,DAY(E41))</f>
@@ -2361,7 +2361,7 @@
         <v>43862</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G42" s="1">
         <f>DATE(YEAR(E42)+1,MONTH(E42),DAY(E42))</f>
@@ -2386,7 +2386,7 @@
         <v>43831</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G43" s="1">
         <f>DATE(YEAR(E43),MONTH(E43)+3,DAY(E43))</f>
@@ -2411,7 +2411,7 @@
         <v>43831</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G44" s="1">
         <f>DATE(YEAR(E44),MONTH(E44)+3,DAY(E44))</f>
@@ -2436,7 +2436,7 @@
         <v>43831</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G45" s="1">
         <f>DATE(YEAR(E45),MONTH(E45)+3,DAY(E45))</f>
@@ -2448,20 +2448,20 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>214</v>
+      </c>
+      <c r="B46" t="s">
         <v>215</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" s="7" t="s">
         <v>216</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>217</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="1">
         <v>43770</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" ref="G46:G55" si="2">DATE(YEAR(E46)+1,MONTH(E46),DAY(E46))</f>
@@ -2482,13 +2482,13 @@
         <v>119</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E47" s="1">
         <v>43634</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="2"/>
@@ -2515,7 +2515,7 @@
         <v>43831</v>
       </c>
       <c r="F48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G48" s="1">
         <f t="shared" si="2"/>
@@ -2540,7 +2540,7 @@
         <v>43617</v>
       </c>
       <c r="F49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" si="2"/>
@@ -2561,13 +2561,13 @@
         <v>125</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E50" s="1">
         <v>43734</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G50" s="1">
         <f t="shared" si="2"/>
@@ -2594,7 +2594,7 @@
         <v>43846</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G51" s="1">
         <f t="shared" si="2"/>
@@ -2606,20 +2606,20 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>217</v>
+      </c>
+      <c r="B52" t="s">
         <v>218</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="1">
         <v>43862</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G52" s="1">
         <f t="shared" si="2"/>
@@ -2646,7 +2646,7 @@
         <v>43891</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G53" s="1">
         <f t="shared" si="2"/>
@@ -2673,7 +2673,7 @@
         <v>43627</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" si="2"/>
@@ -2700,7 +2700,7 @@
         <v>43627</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" si="2"/>
@@ -2727,7 +2727,7 @@
         <v>43885</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G56" s="1">
         <f>DATE(YEAR(E56),MONTH(E56)+3,DAY(E56))</f>
@@ -2739,22 +2739,22 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B57" t="s">
         <v>138</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E57" s="1">
         <v>43435</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H57">
         <v>2018</v>
@@ -2777,7 +2777,7 @@
         <v>43447</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H58">
         <v>2018</v>
@@ -2800,7 +2800,7 @@
         <v>43891</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G59" s="1">
         <f>DATE(YEAR(E59)+1,MONTH(E59),DAY(E59))</f>
@@ -2821,13 +2821,13 @@
         <v>145</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E60" s="1">
         <v>43734</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G60" s="1">
         <f>DATE(YEAR(E60)+1,MONTH(E60),DAY(E60))</f>
@@ -2854,7 +2854,7 @@
         <v>43611</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G61" s="1">
         <f>DATE(YEAR(E61)+1,MONTH(E61),DAY(E61))</f>
@@ -2881,7 +2881,7 @@
         <v>43859</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G62" s="1">
         <v>43950</v>
@@ -2905,7 +2905,7 @@
         <v>43859</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G63" s="1">
         <v>43950</v>
@@ -2931,7 +2931,7 @@
         <v>43831</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G64" s="1">
         <f>DATE(YEAR(E64)+1,MONTH(E64),DAY(E64))</f>
@@ -2958,7 +2958,7 @@
         <v>43859</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G65" s="1">
         <v>43950</v>

</xml_diff>

<commit_message>
Renewable Fuels in Transport Update
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48530ed5e3c44a15/Documents/GitHub/Scottish-Energy-Statistics-Hub/Structure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{6A55E799-6761-4A8D-9CC6-7690E84C63E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D05F11E6-E1EF-4BA8-ACC6-20877066EFC9}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{6A55E799-6761-4A8D-9CC6-7690E84C63E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E6C572C6-FBDD-4A55-902B-047DEB0D1469}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="15855" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,9 +519,6 @@
     <t>https://www.ofgem.gov.uk/</t>
   </si>
   <si>
-    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/863631/2019-third-provisional-rf-01-rtfo-tables.ods</t>
-  </si>
-  <si>
     <t>DFTRenewable</t>
   </si>
   <si>
@@ -775,6 +772,9 @@
   </si>
   <si>
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/868762/LSOA_domestic_elec_2010-18.xlsx</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/883181/2019-fourth-provisional-rf-01-rtfo-tables.ods</t>
   </si>
 </sst>
 </file>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1300,10 +1300,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" t="s">
         <v>167</v>
-      </c>
-      <c r="D1" t="s">
-        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1312,7 +1312,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -1326,16 +1326,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E2" s="1">
         <v>43916</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="1">
         <f>DATE(YEAR(E2),MONTH(E2)+3,DAY(E2))</f>
@@ -1353,16 +1353,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E3" s="1">
         <v>43916</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G3" s="1">
         <f>DATE(YEAR(E3),MONTH(E3)+3,DAY(E3))</f>
@@ -1383,13 +1383,13 @@
         <v>11</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E4" s="1">
         <v>43734</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ref="G4:G10" si="0">DATE(YEAR(E4)+1,MONTH(E4),DAY(E4))</f>
@@ -1410,13 +1410,13 @@
         <v>14</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E5" s="1">
         <v>43647</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
@@ -1437,13 +1437,13 @@
         <v>17</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E6" s="1">
         <v>43647</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
@@ -1464,13 +1464,13 @@
         <v>20</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E7" s="1">
         <v>43647</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
@@ -1491,13 +1491,13 @@
         <v>23</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E8" s="1">
         <v>43647</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
@@ -1509,22 +1509,22 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>224</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>225</v>
       </c>
       <c r="E9" s="11">
         <v>43862</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G9" s="11">
         <f t="shared" si="0"/>
@@ -1545,13 +1545,13 @@
         <v>26</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E10" s="1">
         <v>43800</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
@@ -1575,7 +1575,7 @@
         <v>43916</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H11">
         <v>2018</v>
@@ -1592,13 +1592,13 @@
         <v>32</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E12" s="1">
         <v>43818</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G12" s="1">
         <f>DATE(YEAR(E12)+1,MONTH(E12),DAY(E12))</f>
@@ -1623,7 +1623,7 @@
         <v>43466</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13">
@@ -1638,16 +1638,16 @@
         <v>36</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E14" s="1">
         <v>43862</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G14" s="1">
         <f>DATE(YEAR(E14),MONTH(E14)+3,DAY(E14))</f>
@@ -1665,16 +1665,16 @@
         <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E15" s="1">
         <v>43916</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G15" s="1">
         <f>DATE(YEAR(E15),MONTH(E15)+3,DAY(E15))</f>
@@ -1695,13 +1695,13 @@
         <v>41</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E16" s="1">
         <v>43622</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G16" s="1">
         <f>DATE(YEAR(E16)+1,MONTH(E16),DAY(E16))</f>
@@ -1722,13 +1722,13 @@
         <v>44</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E17" s="1">
         <v>43643</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G17" s="1">
         <f>DATE(YEAR(E17)+1,MONTH(E17),DAY(E17))</f>
@@ -1749,13 +1749,13 @@
         <v>47</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E18" s="1">
         <v>43800</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G18" s="1">
         <f>DATE(YEAR(E18)+1,MONTH(E18),DAY(E18))</f>
@@ -1776,13 +1776,13 @@
         <v>50</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E19" s="1">
         <v>43888</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" ref="G19:G25" si="1">DATE(YEAR(E19),MONTH(E19)+3,DAY(E19))</f>
@@ -1800,16 +1800,16 @@
         <v>52</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E20" s="1">
         <v>43916</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="1"/>
@@ -1827,16 +1827,16 @@
         <v>54</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E21" s="1">
         <v>43916</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="1"/>
@@ -1854,16 +1854,16 @@
         <v>56</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E22" s="1">
         <v>43916</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="1"/>
@@ -1881,16 +1881,16 @@
         <v>58</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E23" s="1">
         <v>43916</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="1"/>
@@ -1908,16 +1908,16 @@
         <v>60</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E24" s="1">
         <v>43916</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="1"/>
@@ -1935,16 +1935,16 @@
         <v>62</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E25" s="1">
         <v>43922</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="1"/>
@@ -1962,16 +1962,16 @@
         <v>64</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E26" s="1">
         <v>43922</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G26" s="1">
         <f>DATE(YEAR(E26),MONTH(E26)+1,DAY(E26))</f>
@@ -1992,13 +1992,13 @@
         <v>67</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E27" s="1">
         <v>43800</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G27" s="1">
         <f>DATE(YEAR(E27)+1,MONTH(E27),DAY(E27))</f>
@@ -2019,13 +2019,13 @@
         <v>70</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E28" s="1">
         <v>43709</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G28" s="1">
         <f>DATE(YEAR(E28)+1,MONTH(E28),DAY(E28))</f>
@@ -2046,13 +2046,13 @@
         <v>73</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E29" s="1">
         <v>43734</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G29" s="1">
         <f>DATE(YEAR(E29)+1,MONTH(E29),DAY(E29))</f>
@@ -2073,13 +2073,13 @@
         <v>32</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E30" s="1">
         <v>43800</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G30" s="1">
         <f>DATE(YEAR(E30)+1,MONTH(E30),DAY(E30))</f>
@@ -2100,13 +2100,13 @@
         <v>78</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E31" s="1">
         <v>43647</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G31" s="1">
         <f>DATE(YEAR(E31)+1,MONTH(E31),DAY(E31))</f>
@@ -2127,13 +2127,13 @@
         <v>81</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E32" s="1">
         <v>43891</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G32" s="1">
         <f>DATE(YEAR(E32),MONTH(E32)+3,DAY(E32))</f>
@@ -2154,13 +2154,13 @@
         <v>84</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E33" s="1">
         <v>43892</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G33" s="1">
         <f>DATE(YEAR(E33),MONTH(E33)+3,DAY(E33))</f>
@@ -2181,13 +2181,13 @@
         <v>87</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E34" s="1">
         <v>43800</v>
       </c>
       <c r="F34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G34" s="1">
         <v>43922</v>
@@ -2198,26 +2198,26 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" t="s">
         <v>163</v>
       </c>
-      <c r="B35" t="s">
-        <v>164</v>
-      </c>
       <c r="C35" s="6" t="s">
-        <v>162</v>
+        <v>247</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E35" s="1">
-        <v>43862</v>
+        <v>43958</v>
       </c>
       <c r="F35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G35" s="1">
         <f>DATE(YEAR(E35),MONTH(E35)+3,DAY(E35))</f>
-        <v>43952</v>
+        <v>44050</v>
       </c>
       <c r="H35">
         <v>2019</v>
@@ -2234,13 +2234,13 @@
         <v>90</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E36" s="1">
         <v>43800</v>
       </c>
       <c r="F36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G36" s="1">
         <v>43922</v>
@@ -2260,13 +2260,13 @@
         <v>93</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E37" s="1">
         <v>43916</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G37" s="1">
         <f>DATE(YEAR(E37),MONTH(E37)+1,DAY(E37))</f>
@@ -2284,7 +2284,7 @@
         <v>95</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>96</v>
@@ -2293,7 +2293,7 @@
         <v>43831</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G38" s="1">
         <f>DATE(YEAR(E38)+1,MONTH(E38),DAY(E38))</f>
@@ -2314,13 +2314,13 @@
         <v>99</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E39" s="1">
         <v>43831</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G39" s="1">
         <f>DATE(YEAR(E39)+1,MONTH(E39),DAY(E39))</f>
@@ -2341,13 +2341,13 @@
         <v>102</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E40" s="1">
         <v>43739</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G40" s="1">
         <f>DATE(YEAR(E40)+1,MONTH(E40),DAY(E40))</f>
@@ -2368,13 +2368,13 @@
         <v>105</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E41" s="1">
         <v>43831</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G41" s="1">
         <f>DATE(YEAR(E41),MONTH(E41)+3,DAY(E41))</f>
@@ -2399,7 +2399,7 @@
         <v>43862</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G42" s="1">
         <f>DATE(YEAR(E42)+1,MONTH(E42),DAY(E42))</f>
@@ -2424,7 +2424,7 @@
         <v>43831</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G43" s="1">
         <f>DATE(YEAR(E43),MONTH(E43)+3,DAY(E43))</f>
@@ -2449,7 +2449,7 @@
         <v>43831</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G44" s="1">
         <f>DATE(YEAR(E44),MONTH(E44)+3,DAY(E44))</f>
@@ -2474,7 +2474,7 @@
         <v>43831</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G45" s="1">
         <f>DATE(YEAR(E45),MONTH(E45)+3,DAY(E45))</f>
@@ -2486,20 +2486,20 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>213</v>
+      </c>
+      <c r="B46" t="s">
         <v>214</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="1">
         <v>43770</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" ref="G46:G55" si="2">DATE(YEAR(E46)+1,MONTH(E46),DAY(E46))</f>
@@ -2520,13 +2520,13 @@
         <v>119</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E47" s="1">
         <v>43634</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="2"/>
@@ -2553,7 +2553,7 @@
         <v>43831</v>
       </c>
       <c r="F48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G48" s="1">
         <f t="shared" si="2"/>
@@ -2578,7 +2578,7 @@
         <v>43617</v>
       </c>
       <c r="F49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" si="2"/>
@@ -2599,13 +2599,13 @@
         <v>125</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E50" s="1">
         <v>43734</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G50" s="1">
         <f t="shared" si="2"/>
@@ -2626,13 +2626,13 @@
         <v>128</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E51" s="1">
         <v>43846</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G51" s="1">
         <f t="shared" si="2"/>
@@ -2644,20 +2644,20 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>216</v>
+      </c>
+      <c r="B52" t="s">
         <v>217</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>219</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="1">
         <v>43862</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G52" s="1">
         <f t="shared" si="2"/>
@@ -2669,22 +2669,22 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" t="s">
         <v>165</v>
-      </c>
-      <c r="B53" t="s">
-        <v>166</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>142</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E53" s="1">
         <v>43891</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G53" s="1">
         <f t="shared" si="2"/>
@@ -2705,13 +2705,13 @@
         <v>131</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E54" s="1">
         <v>43627</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" si="2"/>
@@ -2732,13 +2732,13 @@
         <v>134</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E55" s="1">
         <v>43627</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" si="2"/>
@@ -2756,16 +2756,16 @@
         <v>136</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E56" s="1">
         <v>43885</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G56" s="1">
         <f>DATE(YEAR(E56),MONTH(E56)+3,DAY(E56))</f>
@@ -2777,22 +2777,22 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B57" t="s">
         <v>138</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E57" s="1">
         <v>43435</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H57">
         <v>2018</v>
@@ -2809,13 +2809,13 @@
         <v>139</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E58" s="1">
         <v>43447</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H58">
         <v>2018</v>
@@ -2832,13 +2832,13 @@
         <v>142</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E59" s="1">
         <v>43891</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G59" s="1">
         <f>DATE(YEAR(E59)+1,MONTH(E59),DAY(E59))</f>
@@ -2859,13 +2859,13 @@
         <v>145</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E60" s="1">
         <v>43734</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G60" s="1">
         <f>DATE(YEAR(E60)+1,MONTH(E60),DAY(E60))</f>
@@ -2886,13 +2886,13 @@
         <v>148</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E61" s="1">
         <v>43611</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G61" s="1">
         <f>DATE(YEAR(E61)+1,MONTH(E61),DAY(E61))</f>
@@ -2913,13 +2913,13 @@
         <v>151</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E62" s="1">
         <v>43859</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G62" s="1">
         <v>43950</v>
@@ -2943,7 +2943,7 @@
         <v>43859</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G63" s="1">
         <v>43950</v>
@@ -2963,13 +2963,13 @@
         <v>156</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E64" s="1">
         <v>43831</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G64" s="1">
         <f>DATE(YEAR(E64)+1,MONTH(E64),DAY(E64))</f>
@@ -2990,13 +2990,13 @@
         <v>159</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E65" s="1">
         <v>43859</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G65" s="1">
         <v>43950</v>
@@ -3007,16 +3007,16 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>237</v>
+      </c>
+      <c r="B66" t="s">
         <v>238</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D66" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="E66" s="13">
         <v>43546</v>
@@ -3024,34 +3024,34 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B67" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D67" s="6"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>245</v>
+      </c>
+      <c r="B68" t="s">
+        <v>244</v>
+      </c>
+      <c r="C68" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="B68" t="s">
-        <v>245</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>247</v>
-      </c>
       <c r="D68" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E68" s="1">
         <v>43889</v>
       </c>
       <c r="F68" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G68" s="1">
         <f>DATE(YEAR(E68)+1,MONTH(E68),DAY(E68))</f>

</xml_diff>